<commit_message>
NLP model select done
</commit_message>
<xml_diff>
--- a/corpus_words/corpus_new.xlsx
+++ b/corpus_words/corpus_new.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://soochowmss-my.sharepoint.com/personal/05151330_mss_scu_edu_tw/Documents/python_coding/課程/ccClub/期末專案/財經新聞爬蟲/NLP/corpus_words/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TibeMe_user\Desktop\NLP\corpus_words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="744" documentId="8_{21FABF24-14D1-4791-B736-8B6FA1A845E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23A1A5A6-30F6-4F2D-B14F-0DBC90E79078}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4240E7F1-B3C5-429C-BD0E-6023EC696470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5A22A67-1CC2-4BEE-9BA1-6075A6169D83}"/>
+    <workbookView xWindow="5340" yWindow="444" windowWidth="17280" windowHeight="8964" xr2:uid="{F5A22A67-1CC2-4BEE-9BA1-6075A6169D83}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="1863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2164" uniqueCount="1933">
   <si>
     <t>comment</t>
   </si>
@@ -5951,6 +5951,216 @@
   <si>
     <t>菜色多樣化</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鮭魚很好吃</t>
+  </si>
+  <si>
+    <t>鮭魚很棒</t>
+  </si>
+  <si>
+    <t>鮭魚一般</t>
+  </si>
+  <si>
+    <t>鮭魚難吃</t>
+  </si>
+  <si>
+    <t>鮭魚很難吃</t>
+  </si>
+  <si>
+    <t>鮭魚超級難吃</t>
+  </si>
+  <si>
+    <t>雞腿肉很好吃</t>
+  </si>
+  <si>
+    <t>雞腿肉很棒</t>
+  </si>
+  <si>
+    <t>雞腿肉一般</t>
+  </si>
+  <si>
+    <t>雞腿肉難吃</t>
+  </si>
+  <si>
+    <t>雞腿肉很難吃</t>
+  </si>
+  <si>
+    <t>雞腿肉超級難吃</t>
+  </si>
+  <si>
+    <t>排骨一般</t>
+  </si>
+  <si>
+    <t>排骨難吃</t>
+  </si>
+  <si>
+    <t>排骨很難吃</t>
+  </si>
+  <si>
+    <t>排骨超級難吃</t>
+  </si>
+  <si>
+    <t>香腸很好吃</t>
+  </si>
+  <si>
+    <t>香腸很棒</t>
+  </si>
+  <si>
+    <t>香腸一般</t>
+  </si>
+  <si>
+    <t>香腸難吃</t>
+  </si>
+  <si>
+    <t>香腸很難吃</t>
+  </si>
+  <si>
+    <t>香腸超級難吃</t>
+  </si>
+  <si>
+    <t>綠花椰菜很好吃</t>
+  </si>
+  <si>
+    <t>綠花椰菜很棒</t>
+  </si>
+  <si>
+    <t>綠花椰菜一般</t>
+  </si>
+  <si>
+    <t>綠花椰菜難吃</t>
+  </si>
+  <si>
+    <t>綠花椰菜很難吃</t>
+  </si>
+  <si>
+    <t>綠花椰菜超級難吃</t>
+  </si>
+  <si>
+    <t>滷蛋很好吃</t>
+  </si>
+  <si>
+    <t>滷蛋很棒</t>
+  </si>
+  <si>
+    <t>滷蛋一般</t>
+  </si>
+  <si>
+    <t>滷蛋難吃</t>
+  </si>
+  <si>
+    <t>滷蛋很難吃</t>
+  </si>
+  <si>
+    <t>滷蛋超級難吃</t>
+  </si>
+  <si>
+    <t>荷包蛋很好吃</t>
+  </si>
+  <si>
+    <t>荷包蛋很棒</t>
+  </si>
+  <si>
+    <t>荷包蛋一般</t>
+  </si>
+  <si>
+    <t>荷包蛋難吃</t>
+  </si>
+  <si>
+    <t>荷包蛋很難吃</t>
+  </si>
+  <si>
+    <t>荷包蛋超級難吃</t>
+  </si>
+  <si>
+    <t>豆芽菜很好吃</t>
+  </si>
+  <si>
+    <t>豆芽菜很棒</t>
+  </si>
+  <si>
+    <t>豆芽菜一般</t>
+  </si>
+  <si>
+    <t>豆芽菜難吃</t>
+  </si>
+  <si>
+    <t>豆芽菜很難吃</t>
+  </si>
+  <si>
+    <t>豆芽菜超級難吃</t>
+  </si>
+  <si>
+    <t>番茄很好吃</t>
+  </si>
+  <si>
+    <t>番茄很棒</t>
+  </si>
+  <si>
+    <t>番茄一般</t>
+  </si>
+  <si>
+    <t>番茄難吃</t>
+  </si>
+  <si>
+    <t>番茄很難吃</t>
+  </si>
+  <si>
+    <t>番茄超級難吃</t>
+  </si>
+  <si>
+    <t>青椒很好吃</t>
+  </si>
+  <si>
+    <t>青椒很棒</t>
+  </si>
+  <si>
+    <t>青椒一般</t>
+  </si>
+  <si>
+    <t>青椒難吃</t>
+  </si>
+  <si>
+    <t>青椒很難吃</t>
+  </si>
+  <si>
+    <t>青椒超級難吃</t>
+  </si>
+  <si>
+    <t>茄子很好吃</t>
+  </si>
+  <si>
+    <t>茄子很棒</t>
+  </si>
+  <si>
+    <t>茄子一般</t>
+  </si>
+  <si>
+    <t>茄子難吃</t>
+  </si>
+  <si>
+    <t>茄子很難吃</t>
+  </si>
+  <si>
+    <t>茄子超級難吃</t>
+  </si>
+  <si>
+    <t>四季豆很好吃</t>
+  </si>
+  <si>
+    <t>四季豆很棒</t>
+  </si>
+  <si>
+    <t>四季豆一般</t>
+  </si>
+  <si>
+    <t>四季豆難吃</t>
+  </si>
+  <si>
+    <t>四季豆很難吃</t>
+  </si>
+  <si>
+    <t>四季豆超級難吃</t>
   </si>
 </sst>
 </file>
@@ -6017,7 +6227,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -6033,6 +6243,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -6349,10 +6562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5427935-D6AA-48E1-A492-25F76DF74149}">
-  <dimension ref="A1:E2091"/>
+  <dimension ref="A1:E2163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A2087" workbookViewId="0">
+      <selection activeCell="A2092" sqref="A2092:B2163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -23130,6 +23343,582 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2092" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2092" s="7" t="s">
+        <v>1863</v>
+      </c>
+      <c r="B2092" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2093" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2093" s="7" t="s">
+        <v>1864</v>
+      </c>
+      <c r="B2093" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2094" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2094" s="7" t="s">
+        <v>1865</v>
+      </c>
+      <c r="B2094" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2095" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2095" s="7" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B2095" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2096" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2096" s="7" t="s">
+        <v>1867</v>
+      </c>
+      <c r="B2096" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2097" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2097" s="7" t="s">
+        <v>1868</v>
+      </c>
+      <c r="B2097" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2098" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2098" s="7" t="s">
+        <v>1869</v>
+      </c>
+      <c r="B2098" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2099" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2099" s="7" t="s">
+        <v>1870</v>
+      </c>
+      <c r="B2099" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2100" s="7" t="s">
+        <v>1871</v>
+      </c>
+      <c r="B2100" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2101" s="7" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B2101" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2102" s="7" t="s">
+        <v>1873</v>
+      </c>
+      <c r="B2102" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2103" s="7" t="s">
+        <v>1874</v>
+      </c>
+      <c r="B2103" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2104" s="7" t="s">
+        <v>886</v>
+      </c>
+      <c r="B2104" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2105" s="7" t="s">
+        <v>994</v>
+      </c>
+      <c r="B2105" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2106" s="7" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B2106" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2107" s="7" t="s">
+        <v>1876</v>
+      </c>
+      <c r="B2107" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2108" s="7" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B2108" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2109" s="7" t="s">
+        <v>1878</v>
+      </c>
+      <c r="B2109" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2110" s="7" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B2110" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2111" s="7" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B2111" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2112" s="7" t="s">
+        <v>1881</v>
+      </c>
+      <c r="B2112" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2113" s="7" t="s">
+        <v>1882</v>
+      </c>
+      <c r="B2113" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2114" s="7" t="s">
+        <v>1883</v>
+      </c>
+      <c r="B2114" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2115" s="7" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B2115" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2116" s="7" t="s">
+        <v>1885</v>
+      </c>
+      <c r="B2116" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2117" s="7" t="s">
+        <v>1886</v>
+      </c>
+      <c r="B2117" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2118" s="7" t="s">
+        <v>1887</v>
+      </c>
+      <c r="B2118" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2119" s="7" t="s">
+        <v>1888</v>
+      </c>
+      <c r="B2119" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2120" s="7" t="s">
+        <v>1889</v>
+      </c>
+      <c r="B2120" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2121" s="7" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B2121" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2122" s="7" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B2122" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2123" s="7" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B2123" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2124" s="7" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B2124" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2125" s="7" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B2125" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2126" s="7" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B2126" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2127" s="7" t="s">
+        <v>1896</v>
+      </c>
+      <c r="B2127" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2128" s="7" t="s">
+        <v>1897</v>
+      </c>
+      <c r="B2128" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2129" s="7" t="s">
+        <v>1898</v>
+      </c>
+      <c r="B2129" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2130" s="7" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B2130" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2131" s="7" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B2131" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2132" s="7" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B2132" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2133" s="7" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B2133" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2134" s="7" t="s">
+        <v>1903</v>
+      </c>
+      <c r="B2134" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2135" s="7" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B2135" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2136" s="7" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B2136" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2137" s="7" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B2137" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2138" s="7" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B2138" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2139" s="7" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B2139" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2140" s="7" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B2140" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2141" s="7" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B2141" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2142" s="7" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B2142" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2143" s="7" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B2143" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2144" s="7" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B2144" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2145" s="7" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B2145" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2146" s="7" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B2146" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2147" s="7" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B2147" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2148" s="7" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B2148" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2149" s="7" t="s">
+        <v>1918</v>
+      </c>
+      <c r="B2149" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2150" s="7" t="s">
+        <v>1919</v>
+      </c>
+      <c r="B2150" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2151" s="7" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B2151" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2152" s="7" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B2152" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2153" s="7" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B2153" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2154" s="7" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B2154" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2155" s="7" t="s">
+        <v>1924</v>
+      </c>
+      <c r="B2155" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2156" s="7" t="s">
+        <v>1925</v>
+      </c>
+      <c r="B2156" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2157" s="7" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B2157" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2158" s="7" t="s">
+        <v>1927</v>
+      </c>
+      <c r="B2158" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2159" s="7" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B2159" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2160" s="7" t="s">
+        <v>1929</v>
+      </c>
+      <c r="B2160" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2161" s="7" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B2161" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2162" s="7" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B2162" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2163" s="7" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B2163" s="7">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B2091">
     <sortCondition ref="A2:A2091"/>

</xml_diff>